<commit_message>
Updating the leetcode excel
</commit_message>
<xml_diff>
--- a/leetcode/Leetcode-progress.xlsx
+++ b/leetcode/Leetcode-progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rahulmr96\ut-austin\mis385_rmr3923\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D486131-5F71-46A1-9977-726188234BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019401DE-90B0-47A9-A43D-BFF90F8D61D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6AFBCFA4-A149-4AA2-87C5-B265FA407B29}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D107"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>